<commit_message>
choix composants + bonde commande
</commit_message>
<xml_diff>
--- a/Composants/Bon de commande.xlsx
+++ b/Composants/Bon de commande.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Désignation et référence constructeur</t>
   </si>
@@ -47,30 +47,12 @@
     <t>Lien</t>
   </si>
   <si>
-    <t>http://www.futurheli.com/fr/4053-helice-12-x-8-electrique-propulsive-apc-.html</t>
-  </si>
-  <si>
     <t>Grande hélice de propulsion - HFL7766</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>futurheli</t>
-  </si>
-  <si>
-    <t>http://www.euromodel-online.eu/pro-tronik-moteur-dm2625-900kv.html</t>
-  </si>
-  <si>
-    <t>euromodel</t>
-  </si>
-  <si>
-    <t>PRO72625</t>
-  </si>
-  <si>
-    <t>Grand moteur - DM2625 900Kv</t>
-  </si>
-  <si>
     <t>http://www.envergure-modelisme.fr/moteurs-electriques/3305-moteur-ray-cdr-cd3536-05.html</t>
   </si>
   <si>
@@ -80,24 +62,6 @@
     <t>Petit moteur - RAY CDR CD3536/05</t>
   </si>
   <si>
-    <t>http://www.jjmstore.fr/skysport-40-40a-2-3s-bec-rcplus-rcsks040b.html</t>
-  </si>
-  <si>
-    <t>jjmstore</t>
-  </si>
-  <si>
-    <t>Contrôleur - SKYSPORT 40 40A - 2-3S - BEC - RcPlus - rcsks040b</t>
-  </si>
-  <si>
-    <t>Servo moteur</t>
-  </si>
-  <si>
-    <t>http://letmeknow.fr/shop/moteur/30-servo-moteur-nano-4894479459935.html</t>
-  </si>
-  <si>
-    <t>letmeknow</t>
-  </si>
-  <si>
     <t>Accéléromètre - SEN0032</t>
   </si>
   <si>
@@ -111,6 +75,33 @@
   </si>
   <si>
     <t>gotronic</t>
+  </si>
+  <si>
+    <t>http://www.gotronic.fr/art-servomoteur-sg90-19377.htm</t>
+  </si>
+  <si>
+    <t>Servo moteur - SG90</t>
+  </si>
+  <si>
+    <t>Variateur - SKYSPORT 40 40A - 2-3S - BEC - RcPlus - rcsks040b</t>
+  </si>
+  <si>
+    <t>http://www.miniplanes.fr/electrique-/controleurs-brushless/controleur-brushless-skyport-40-40a-p-45164.html</t>
+  </si>
+  <si>
+    <t>http://www.miniplanes.fr/electrique-/moteurs-brushless/2625-kv-900-a2pro-p-43357.html</t>
+  </si>
+  <si>
+    <t>miniplanes</t>
+  </si>
+  <si>
+    <t>A2P-72625</t>
+  </si>
+  <si>
+    <t>Grand moteur - 2625 / Kv 900 A2PRO</t>
+  </si>
+  <si>
+    <t>http://www.miniplanes.fr/helices-cones/helices-electrique/helice-ep1280-elecflight-12x8-305x203mm-jp4460785-p-5681.html</t>
   </si>
 </sst>
 </file>
@@ -217,9 +208,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -229,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,12 +512,12 @@
     <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="116" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -559,61 +548,61 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8">
-        <v>6.92</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="E4" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="8">
         <f>D4*E4</f>
-        <v>6.92</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D5" s="8">
-        <v>45.5</v>
+        <v>39.9</v>
       </c>
       <c r="E5" s="9">
         <v>1</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" ref="F5:F9" si="0">D5*E5</f>
-        <v>45.5</v>
+        <v>39.9</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" s="7">
         <v>1504004</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" s="8">
         <v>14.5</v>
@@ -626,66 +615,66 @@
         <v>14.5</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="8">
-        <v>18.899999999999999</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="E7" s="9">
         <v>2</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="0"/>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>18</v>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="7">
+        <v>31760</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D8" s="8">
-        <v>3.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B9" s="7">
         <v>32196</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D9" s="8">
         <v>8.5</v>
@@ -698,22 +687,22 @@
         <v>8.5</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="9" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F10" s="8">
         <f>SUM(F4:F9)</f>
-        <v>116.72</v>
-      </c>
-      <c r="G10" s="13"/>
+        <v>111.46000000000001</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>

</xml_diff>